<commit_message>
locators can now be used
</commit_message>
<xml_diff>
--- a/excel_reports/22-08-2022.xlsx
+++ b/excel_reports/22-08-2022.xlsx
@@ -482,15 +482,43 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PASSED</t>
+          <t>FAILED</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>6.336872609000238</v>
+        <v>8.488922890999675</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-08-22T11:42:51</t>
+          <t>2022-08-22T17:37:53</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>selenium.common.exceptions.InvalidArgumentException: Message: invalid argument: 'text' is empty
+  (Session info: chrome=104.0.5112.101)
+Stacktrace:
+0   chromedriver                        0x000000010ece4149 chromedriver + 4469065
+1   chromedriver                        0x000000010ec6e233 chromedriver + 3985971
+2   chromedriver                        0x000000010e904fe8 chromedriver + 409576
+3   chromedriver                        0x000000010e933a78 chromedriver + 600696
+4   chromedriver                        0x000000010e958c62 chromedriver + 752738
+5   chromedriver                        0x000000010e92fe35 chromedriver + 585269
+6   chromedriver                        0x000000010e958d6e chromedriver + 753006
+7   chromedriver                        0x000000010e96b611 chromedriver + 828945
+8   chromedriver                        0x000000010e958b53 chromedriver + 752467
+9   chromedriver                        0x000000010e92e905 chromedriver + 579845
+10  chromedriver                        0x000000010e92f955 chromedriver + 584021
+11  chromedriver                        0x000000010ecb56ad chromedriver + 4277933
+12  chromedriver                        0x000000010ecb9b3a chromedriver + 4295482
+13  chromedriver                        0x000000010ecbecdf chromedriver + 4316383
+14  chromedriver                        0x000000010ecba857 chromedriver + 4298839
+15  chromedriver                        0x000000010ec9364f chromedriver + 4138575
+16  chromedriver                        0x000000010ecd51f8 chromedriver + 4407800
+17  chromedriver                        0x000000010ecd537f chromedriver + 4408191
+18  chromedriver                        0x000000010ecebcb5 chromedriver + 4500661
+19  libsystem_pthread.dylib             0x00007ff80a4144e1 _pthread_start + 125
+20  libsystem_pthread.dylib             0x00007ff80a40ff6b thread_start + 15</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">

</xml_diff>